<commit_message>
Modificar formato de prueba
</commit_message>
<xml_diff>
--- a/Documentos/Formato de prueba.xlsx
+++ b/Documentos/Formato de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Temporal\Desktop\Ingenieria de software\Inventario_escuela\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52E990C-C298-4862-B455-059774CAC6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9356A19-80B6-4830-B865-F4F43CA29988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>PLANTILLA DE PLANIFICACIÓN Y EJECUCIÓN DE CASOS DE PRUEBA</t>
   </si>
@@ -630,12 +630,6 @@
     <t>REPROBAR</t>
   </si>
   <si>
-    <t>Validar el ingreso de caracteres especiales</t>
-  </si>
-  <si>
-    <t>El sistema valida que el campo no este vacio, permite el ingreso de todos los caracteres, valida la longitud máxima</t>
-  </si>
-  <si>
     <t>El sistema toma por defecto el valor de 0 al registrar la sala</t>
   </si>
   <si>
@@ -646,6 +640,15 @@
   </si>
   <si>
     <t>El sistema valida que se selecione un estado</t>
+  </si>
+  <si>
+    <t>El sistema valida que el campo no este vacio, permite el ingreso de todos los caracteres, valida la longitud máxima pero se puede ingresar una cantidad ilimitada de datos</t>
+  </si>
+  <si>
+    <t>Validar el ingreso de caracteres especiales y controlar la cantidad de datos ingresados</t>
+  </si>
+  <si>
+    <t>Validar el ingreso de caracteres especiales  y controlar la cantidad de datos ingresados</t>
   </si>
 </sst>
 </file>
@@ -1416,8 +1419,8 @@
   <dimension ref="A1:EZ919"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15:E35"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1776,13 +1779,13 @@
         <v>86</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G11" s="22" t="s">
         <v>89</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1800,13 +1803,13 @@
         <v>87</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>89</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1824,13 +1827,13 @@
         <v>88</v>
       </c>
       <c r="F13" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="20" t="s">
         <v>92</v>
-      </c>
-      <c r="G13" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1848,10 +1851,10 @@
         <v>32</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H14" s="20"/>
     </row>

</xml_diff>

<commit_message>
Termiando formato de pruebas: Modulo salas
</commit_message>
<xml_diff>
--- a/Documentos/Formato de prueba.xlsx
+++ b/Documentos/Formato de prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Temporal\Desktop\Ingenieria de software\Inventario_escuela\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9356A19-80B6-4830-B865-F4F43CA29988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1E51E9-93D6-4209-B53A-D55A7B1E9D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>PLANTILLA DE PLANIFICACIÓN Y EJECUCIÓN DE CASOS DE PRUEBA</t>
   </si>
@@ -129,187 +129,7 @@
     <t>RF2</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>DESCRIPCIÓN</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>El sistema proporciona una lista desplegable con varios tipos de equipos pre definido, el usuario debe seleccionar un tipo de la lista.</t>
-  </si>
-  <si>
-    <t>El usuario debe ingresar las especificaciones técnicas del equipo dentro de un text-area, las cuales pueden contener, texto, números y caracteres especiales.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>ESPECIFICACIONES TÉCNICAS</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>APLICACIONES</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>El usuario debe ingresar las aplicaciones que contenga el equipo, este campo es opcional, pude quedar vacio en caso de que el equipo no presente aplicaciones, debe ser ingresado dentro de un text-area, las cuales pueden contener, texto, números y caracteres especiales.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El usuario debe ingresar la descripción del equipo, donde también van incluidas novedades que este presente, debe ser ingresado dentro de un text-area, las cuales pueden contener, texto, números y caracteres especiales. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>MODELO.</t>
-    </r>
-  </si>
-  <si>
-    <t>EL usuario debe ingresar el nombre del equipo por entrada (teclado), el cual puede contener números y letras, espacios y caracteres especiales.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>CONFIGURACIÓN DE RED.</t>
-    </r>
-  </si>
-  <si>
-    <t>EL usuario debe ingresar la configuración de red actual del equipo por entrada (teclado), este campo es opcional por si el equipo no presenta una caracteristica de configuración de red. Este campo puede contener números y letras, espacios y caracteres especiales.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>UBICACIÓN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>ESTADO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite registrar los equipos de cada una de las salas de sistemas de la escuela: Verificación datos de entrada </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>FECHA DE REGISTRO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>El sistema proporciona una lista desplegable con los diferentes estados posibles que presenta el equipo. El usuario debe seleccionar un estado de la lista.</t>
-  </si>
-  <si>
-    <t>El sistema proporciona una lista desplegable con las ubicaciones donde deberían estar los de equipos las cuales corresponden a las difrentes salas de sistemas y departamentos. El usuario debe seleccionar una ubicación de la lista.</t>
-  </si>
-  <si>
-    <t>El sistema proporciona un calendario donde se podra seleccionar la fecha de registro del equipo, la cual tendra el formato aaaa-mm-dd. El usuario debe seleccionar una fecha de la lista.</t>
   </si>
   <si>
     <t>RF1.1</t>
@@ -330,190 +150,10 @@
     <t>El sistema valida que los datos proporcionados sean los necesarios de acuerdo a documento de clasificación de datos (tipo, longitud, formulario, características) de acuerdo con el documento de clasificación de datos.</t>
   </si>
   <si>
-    <t>RF1.3</t>
-  </si>
-  <si>
-    <t>Asignación de fotografía.</t>
-  </si>
-  <si>
-    <t>El sistema asigna una fotografía del equipo registrado con formato definido en documento de clasificación de datos, al seleccionar la fotografía solo debe permitir formato JPG.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite consultar los equipos que ya se encuentran registrados por el parametro: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>CONSULTA POR CÓDIGO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite consultar los equipos que ya se encuentran registrados por el parametro: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>CONSULTA POR UBICACIÓN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite consultar los equipos que ya se encuentran registrados por el parametro: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>CONSULTA POR CATEGORÍA.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite consultar los equipos que ya se encuentran registrados por el parametro: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>CONSULTA POR NOMBRE.</t>
-    </r>
-  </si>
-  <si>
-    <t>RF2.1</t>
-  </si>
-  <si>
-    <t>RF2.2</t>
-  </si>
-  <si>
-    <t>RF2.3</t>
-  </si>
-  <si>
-    <t>El usuario puede consultar un equipo en especifico ingresando el código correspondiente al equipo, el tipo de dato debe ser validado de acuerdo al documento de clasificación de datos, si el campo esta vacio ó el tipo de dato es incorrecto el sistema debe mostrar un mensaje indicando al usuario el error.</t>
-  </si>
-  <si>
-    <t>El usuario puede consulta todos los equipos de una categoría especifica ingresando la categoría que desea mapear, el tipo de dato debe ser validado de acuerdo al documento de clasificación de datos, si el campo esta vacio ó el tipo de dato es incorrecto el sistema debe mostrar un mensaje indicando al usuario el error.</t>
-  </si>
-  <si>
-    <t>El usuario puede consulta todos los equipos de una ubicación determinada especifica ingresando la ubicaciión que desea mapear,  el tipo de dato debe ser validado de acuerdo al documento de clasificación de datos, si el campo esta vacio ó el tipo de dato es incorrecto el sistema debe mostrar un mensaje indicando al usuario el error.</t>
-  </si>
-  <si>
-    <t>El usuario puede consultar un equipo en especifico ingresando el nombre correspondiente al equipo, el tipo de dato debe ser validado de acuerdo al documento de clasificación de datos, si el campo esta vacio ó el tipo de dato es incorrecto el sistema debe mostrar un mensaje indicando al usuario el error.</t>
-  </si>
-  <si>
     <t>RF3</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">El sistema permite actualizar la información de los equipos: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>UBICACIÓN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite actualizar la información de los equipos: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>DESCRIPCIÓN.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite actualizar la información de los equipos: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>APLICACIONES.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite actualizar la información de los equipos: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>ESTADO.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">El sistema permite actualizar la información de los equipos: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Century Gothic"/>
-        <family val="2"/>
-      </rPr>
-      <t>ESPECIFICACIONES TECNICAS.</t>
-    </r>
-  </si>
-  <si>
     <t>RF3.1</t>
-  </si>
-  <si>
-    <t>El sistema hace una consulta previa del equipo antes de actualizar, para validar que el equipo que se quiere actualizar si exista, los campos que no se pueden actualizar estaran inhabilitados y los que se pueden actualizar estaran disponibles para su edición.</t>
-  </si>
-  <si>
-    <t>El usuario debe ingresar las especificaciones técnicas del equipo dentro de un text-area, las cuales pueden contener, texto, números y caracteres especiales. En caso de quedar un campo vacio el sistema tomara el valor que tenía previamente el equipo, las caracteristicas de los datos ingresados deben ser validados de acuerdo al documento de clasificación de prueba.</t>
-  </si>
-  <si>
-    <t>El sistema proporciona una lista desplegable con los diferentes estados posibles que presenta el equipo. El usuario debe seleccionar un estado de la lista. En caso de quedar un campo vacio el sistema tomara el valor que tenía previamente el equipo, las caracteristicas de los datos ingresados deben ser validados de acuerdo al documento de clasificación de prueba.</t>
-  </si>
-  <si>
-    <t>El usuario debe ingresar la descripción del equipo, donde también van incluidas novedades que este presente, debe ser ingresado dentro de un text-area, las cuales pueden contener, texto, números y caracteres especiales. En caso de quedar un campo vacio el sistema tomara el valor que tenía previamente el equipo, las caracteristicas de los datos ingresados deben ser validados de acuerdo al documento de clasificación de prueba.</t>
-  </si>
-  <si>
-    <t>El sistema proporciona una lista desplegable con las ubicaciones donde deberían estar los de equipos las cuales corresponden a las difrentes salas de sistemas y departamentos. El usuario debe seleccionar una ubicación de la lista. En caso de quedar un campo vacio el sistema tomara el valor que tenía previamente el equipo, las caracteristicas de los datos ingresados deben ser validados de acuerdo al documento de clasificación de prueba.</t>
   </si>
   <si>
     <t>Modulo de sala</t>
@@ -650,6 +290,99 @@
   <si>
     <t>Validar el ingreso de caracteres especiales  y controlar la cantidad de datos ingresados</t>
   </si>
+  <si>
+    <t>El sistema valida que el equipo ya se encuantra registrado, manda un mensaje indicando que hay problemas con el registro de la sala</t>
+  </si>
+  <si>
+    <t>Especificar en el mensaje cual es el problema con el registro.</t>
+  </si>
+  <si>
+    <t>El sistema valida los datos ingresados según su tipo, longitud, formulario y caracteristicas, y devuelve un mensaje al usuario que indica que hay problemas en el registro de la sala</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El sistema permite consultar las salas que ya se encuentran registrados por el parametro: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>CONSULTA POR CÓDIGO.</t>
+    </r>
+  </si>
+  <si>
+    <t>El usuario puede consultar una sala en especifico ingresando el código correspondiente a la sala, el tipo de dato debe ser validado de acuerdo al documento de clasificación de datos, si el campo esta vacio ó el tipo de dato es incorrecto el sistema debe mostrar un mensaje indicando al usuario el error.</t>
+  </si>
+  <si>
+    <t>El sistema valida que el campo no este vacio, no valida la cantidad de caracteres ingresados ni el tipo, muestra un mensaje de error si el campo esta vacio y también si no encuentra el registro.</t>
+  </si>
+  <si>
+    <t>Validar el tipo y longitud de los caracteres ingresados.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El sistema permite actualizar la información de las salas: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>ESTADO.</t>
+    </r>
+  </si>
+  <si>
+    <t>El sistema proporciona una lista desplegable con los diferentes estados posibles que presentan las salas. El usuario debe seleccionar un estado de la lista. En caso de quedar un campo vacio el sistema tomara el valor que tenía previamente el equipo, las caracteristicas de los datos ingresados deben ser validados de acuerdo al documento de clasificación de prueba.</t>
+  </si>
+  <si>
+    <t>El sistema permite al usuario actualizar una sala previamente consultada, el usuario selecciona el estado de la lista desplegable y previamente le da en actualizar.</t>
+  </si>
+  <si>
+    <t>Deshabilitar el botón actualizar hasta que se consulte una sala.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El sistema permite actualizar la información de las salas: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>NOMBRE SALA.</t>
+    </r>
+  </si>
+  <si>
+    <t>El sistema permite cambiar el valor de la caja de texto correspondiente al nombre de la sala, en caso de que este vacio el sistema toma el valor que previamente tenia, el sistema debe validar la longitud y tipo de caracteres ingresados en la caja de texto.</t>
+  </si>
+  <si>
+    <t>El sistema permite al usuario actualizar el nombre de la sala, no se valida el tipo de dato ni la longitud del campo, el sistema no valida que el campo este vacio y actualiza un valor vacio.</t>
+  </si>
+  <si>
+    <t>Realizar las validaciones en caso de que el campo este vacio, y validar los tipos y longitud de los datos.</t>
+  </si>
+  <si>
+    <t>Valiar la existencia de la sala.</t>
+  </si>
+  <si>
+    <t>El sistema hace una consulta previa de la sala antes de actualizar, para validar que la sala que se quiere actualizar si exista, los campos que no se pueden actualizar estaran inhabilitados y los que se pueden actualizar estaran disponibles para su edición.</t>
+  </si>
+  <si>
+    <t>No se hace consulta previa</t>
+  </si>
+  <si>
+    <t>Deshabilitar el botón actualizar hasta que se consulte una sala, para cumplir este requerimiento.</t>
+  </si>
 </sst>
 </file>
 
@@ -658,7 +391,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -768,13 +501,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -975,7 +701,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1074,7 +800,6 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1416,11 +1141,11 @@
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EZ919"/>
+  <dimension ref="A1:EZ901"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1621,7 +1346,7 @@
       <c r="A3" s="19"/>
       <c r="B3" s="19"/>
       <c r="C3" s="34" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D3" s="26" t="s">
         <v>13</v>
@@ -1665,7 +1390,7 @@
       <c r="A5" s="19"/>
       <c r="B5" s="19"/>
       <c r="C5" s="33" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="27" t="s">
@@ -1770,22 +1495,22 @@
         <v>29</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="D11" s="16">
         <v>45357</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1794,22 +1519,22 @@
         <v>29</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="D12" s="16">
         <v>45357</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1818,22 +1543,22 @@
         <v>29</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D13" s="16">
         <v>45357</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:156" ht="99" x14ac:dyDescent="0.25">
@@ -1842,398 +1567,356 @@
         <v>29</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="D14" s="16">
         <v>45357</v>
       </c>
       <c r="E14" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:156" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>93</v>
+      <c r="C15" s="15" t="s">
+        <v>33</v>
       </c>
-      <c r="G14" s="22" t="s">
-        <v>91</v>
+      <c r="D15" s="16">
+        <v>45358</v>
       </c>
-      <c r="H14" s="20"/>
-    </row>
-    <row r="15" spans="1:156" ht="113.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="15" t="s">
+      <c r="E15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="20" t="s">
-        <v>33</v>
+      <c r="F15" s="21" t="s">
+        <v>57</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="20"/>
-    </row>
-    <row r="16" spans="1:156" ht="135" x14ac:dyDescent="0.25">
+      <c r="G15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:156" ht="108" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="35" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="D16" s="16">
+        <v>45358</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="162" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="16">
+        <v>45358</v>
+      </c>
       <c r="E17" s="20" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="F17" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="189" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="35" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="16">
+        <v>45358</v>
+      </c>
       <c r="E18" s="20" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="20"/>
+      <c r="F18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="35" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
-      <c r="D19" s="16"/>
+      <c r="D19" s="16">
+        <v>45358</v>
+      </c>
       <c r="E19" s="20" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="20"/>
-    </row>
-    <row r="20" spans="1:8" ht="121.5" x14ac:dyDescent="0.25">
+      <c r="F19" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="35" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="16">
+        <v>45358</v>
+      </c>
       <c r="E20" s="20" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="20"/>
-    </row>
-    <row r="21" spans="1:8" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="35" t="s">
-        <v>29</v>
+      <c r="F20" s="21" t="s">
+        <v>74</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="20"/>
-    </row>
-    <row r="22" spans="1:8" ht="108" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="20"/>
-    </row>
-    <row r="23" spans="1:8" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="15" t="s">
+      <c r="G20" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="20"/>
-    </row>
-    <row r="24" spans="1:8" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="20"/>
-    </row>
-    <row r="25" spans="1:8" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="20"/>
-    </row>
-    <row r="26" spans="1:8" ht="178.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="20"/>
-    </row>
-    <row r="27" spans="1:8" ht="189" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" ht="175.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" ht="162" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="20"/>
-    </row>
-    <row r="30" spans="1:8" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" ht="229.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="20"/>
-    </row>
-    <row r="32" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="20"/>
-    </row>
-    <row r="33" spans="1:8" ht="189" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="20"/>
-    </row>
-    <row r="34" spans="1:8" ht="189" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="20"/>
-    </row>
-    <row r="35" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="36"/>
-      <c r="B35" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="20" t="s">
+      <c r="H20" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="20"/>
-    </row>
-    <row r="36" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="35"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="20"/>
-    </row>
-    <row r="37" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="15"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="20"/>
-    </row>
-    <row r="38" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="35"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="20"/>
-    </row>
-    <row r="39" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="37" t="s">
+    </row>
+    <row r="21" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="38"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+    </row>
+    <row r="22" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
@@ -10855,189 +10538,9 @@
       <c r="G901" s="1"/>
       <c r="H901" s="1"/>
     </row>
-    <row r="902" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A902" s="1"/>
-      <c r="B902" s="1"/>
-      <c r="C902" s="1"/>
-      <c r="D902" s="1"/>
-      <c r="E902" s="1"/>
-      <c r="F902" s="1"/>
-      <c r="G902" s="1"/>
-      <c r="H902" s="1"/>
-    </row>
-    <row r="903" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A903" s="1"/>
-      <c r="B903" s="1"/>
-      <c r="C903" s="1"/>
-      <c r="D903" s="1"/>
-      <c r="E903" s="1"/>
-      <c r="F903" s="1"/>
-      <c r="G903" s="1"/>
-      <c r="H903" s="1"/>
-    </row>
-    <row r="904" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A904" s="1"/>
-      <c r="B904" s="1"/>
-      <c r="C904" s="1"/>
-      <c r="D904" s="1"/>
-      <c r="E904" s="1"/>
-      <c r="F904" s="1"/>
-      <c r="G904" s="1"/>
-      <c r="H904" s="1"/>
-    </row>
-    <row r="905" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A905" s="1"/>
-      <c r="B905" s="1"/>
-      <c r="C905" s="1"/>
-      <c r="D905" s="1"/>
-      <c r="E905" s="1"/>
-      <c r="F905" s="1"/>
-      <c r="G905" s="1"/>
-      <c r="H905" s="1"/>
-    </row>
-    <row r="906" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A906" s="1"/>
-      <c r="B906" s="1"/>
-      <c r="C906" s="1"/>
-      <c r="D906" s="1"/>
-      <c r="E906" s="1"/>
-      <c r="F906" s="1"/>
-      <c r="G906" s="1"/>
-      <c r="H906" s="1"/>
-    </row>
-    <row r="907" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A907" s="1"/>
-      <c r="B907" s="1"/>
-      <c r="C907" s="1"/>
-      <c r="D907" s="1"/>
-      <c r="E907" s="1"/>
-      <c r="F907" s="1"/>
-      <c r="G907" s="1"/>
-      <c r="H907" s="1"/>
-    </row>
-    <row r="908" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A908" s="1"/>
-      <c r="B908" s="1"/>
-      <c r="C908" s="1"/>
-      <c r="D908" s="1"/>
-      <c r="E908" s="1"/>
-      <c r="F908" s="1"/>
-      <c r="G908" s="1"/>
-      <c r="H908" s="1"/>
-    </row>
-    <row r="909" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A909" s="1"/>
-      <c r="B909" s="1"/>
-      <c r="C909" s="1"/>
-      <c r="D909" s="1"/>
-      <c r="E909" s="1"/>
-      <c r="F909" s="1"/>
-      <c r="G909" s="1"/>
-      <c r="H909" s="1"/>
-    </row>
-    <row r="910" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A910" s="1"/>
-      <c r="B910" s="1"/>
-      <c r="C910" s="1"/>
-      <c r="D910" s="1"/>
-      <c r="E910" s="1"/>
-      <c r="F910" s="1"/>
-      <c r="G910" s="1"/>
-      <c r="H910" s="1"/>
-    </row>
-    <row r="911" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A911" s="1"/>
-      <c r="B911" s="1"/>
-      <c r="C911" s="1"/>
-      <c r="D911" s="1"/>
-      <c r="E911" s="1"/>
-      <c r="F911" s="1"/>
-      <c r="G911" s="1"/>
-      <c r="H911" s="1"/>
-    </row>
-    <row r="912" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A912" s="1"/>
-      <c r="B912" s="1"/>
-      <c r="C912" s="1"/>
-      <c r="D912" s="1"/>
-      <c r="E912" s="1"/>
-      <c r="F912" s="1"/>
-      <c r="G912" s="1"/>
-      <c r="H912" s="1"/>
-    </row>
-    <row r="913" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A913" s="1"/>
-      <c r="B913" s="1"/>
-      <c r="C913" s="1"/>
-      <c r="D913" s="1"/>
-      <c r="E913" s="1"/>
-      <c r="F913" s="1"/>
-      <c r="G913" s="1"/>
-      <c r="H913" s="1"/>
-    </row>
-    <row r="914" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A914" s="1"/>
-      <c r="B914" s="1"/>
-      <c r="C914" s="1"/>
-      <c r="D914" s="1"/>
-      <c r="E914" s="1"/>
-      <c r="F914" s="1"/>
-      <c r="G914" s="1"/>
-      <c r="H914" s="1"/>
-    </row>
-    <row r="915" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A915" s="1"/>
-      <c r="B915" s="1"/>
-      <c r="C915" s="1"/>
-      <c r="D915" s="1"/>
-      <c r="E915" s="1"/>
-      <c r="F915" s="1"/>
-      <c r="G915" s="1"/>
-      <c r="H915" s="1"/>
-    </row>
-    <row r="916" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A916" s="1"/>
-      <c r="B916" s="1"/>
-      <c r="C916" s="1"/>
-      <c r="D916" s="1"/>
-      <c r="E916" s="1"/>
-      <c r="F916" s="1"/>
-      <c r="G916" s="1"/>
-      <c r="H916" s="1"/>
-    </row>
-    <row r="917" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A917" s="1"/>
-      <c r="B917" s="1"/>
-      <c r="C917" s="1"/>
-      <c r="D917" s="1"/>
-      <c r="E917" s="1"/>
-      <c r="F917" s="1"/>
-      <c r="G917" s="1"/>
-      <c r="H917" s="1"/>
-    </row>
-    <row r="918" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A918" s="1"/>
-      <c r="B918" s="1"/>
-      <c r="C918" s="1"/>
-      <c r="D918" s="1"/>
-      <c r="E918" s="1"/>
-      <c r="F918" s="1"/>
-      <c r="G918" s="1"/>
-      <c r="H918" s="1"/>
-    </row>
-    <row r="919" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A919" s="1"/>
-      <c r="B919" s="1"/>
-      <c r="C919" s="1"/>
-      <c r="D919" s="1"/>
-      <c r="E919" s="1"/>
-      <c r="F919" s="1"/>
-      <c r="G919" s="1"/>
-      <c r="H919" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B21:H21"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <conditionalFormatting sqref="D3">
@@ -11057,7 +10560,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>

</xml_diff>

<commit_message>
Test de formato de prueba y Actualización de formato de prueba
</commit_message>
<xml_diff>
--- a/Documentos/Formato de prueba.xlsx
+++ b/Documentos/Formato de prueba.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Temporal\Desktop\Ingenieria de software\Inventario_escuela\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9A3AC5-6261-4958-B1BD-A61B7FC1E40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A23F39-6071-41F8-ACA8-8E2675361A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato de prueba - Modulo sala" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
   <si>
     <t>PLANTILLA DE PLANIFICACIÓN Y EJECUCIÓN DE CASOS DE PRUEBA</t>
   </si>
@@ -868,6 +868,9 @@
   <si>
     <t>Modulo de registro equipos</t>
   </si>
+  <si>
+    <t>Dulfran Montaño Montaño</t>
+  </si>
 </sst>
 </file>
 
@@ -1292,11 +1295,11 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1667,9 +1670,9 @@
   </sheetPr>
   <dimension ref="A1:EZ901"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N44" sqref="N44"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1920,7 +1923,9 @@
       <c r="E5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="27" t="s">
+        <v>127</v>
+      </c>
       <c r="G5" s="28">
         <v>45357</v>
       </c>
@@ -2252,15 +2257,15 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
     </row>
     <row r="22" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -11100,9 +11105,9 @@
   </sheetPr>
   <dimension ref="A1:EZ919"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11353,7 +11358,9 @@
       <c r="E5" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="27" t="s">
+        <v>127</v>
+      </c>
       <c r="G5" s="28" t="s">
         <v>125</v>
       </c>
@@ -11831,7 +11838,7 @@
       <c r="H34" s="20"/>
     </row>
     <row r="35" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A35" s="38"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="35" t="s">
         <v>39</v>
       </c>
@@ -11877,15 +11884,15 @@
       <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
     </row>
     <row r="40" spans="1:8" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>

</xml_diff>